<commit_message>
puit à colonne permanente
</commit_message>
<xml_diff>
--- a/éléments de construction/spécification.xlsx
+++ b/éléments de construction/spécification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="64320" yWindow="-940" windowWidth="25600" windowHeight="14760" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="montage financier" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="domoti" sheetId="4" r:id="rId4"/>
     <sheet name="contacts" sheetId="5" r:id="rId5"/>
     <sheet name="Géothermie" sheetId="6" r:id="rId6"/>
-    <sheet name="Feuil1" sheetId="7" r:id="rId7"/>
+    <sheet name="cuisine" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="90">
   <si>
     <t xml:space="preserve">Hypothèque  </t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>10% par trance de 1000$ à partir du mois du 7 mars 2016 au 18 avril 2016</t>
+  </si>
+  <si>
+    <t>http://www.ecohabitation.com/actualite/nouvelles/comprendre-geothermie</t>
+  </si>
+  <si>
+    <t>pcp - puits à colonne permanente</t>
   </si>
 </sst>
 </file>
@@ -1451,27 +1457,35 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1491,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>